<commit_message>
Little Update on the file
</commit_message>
<xml_diff>
--- a/Backend/Brands.xlsx
+++ b/Backend/Brands.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhtw-my.sharepoint.com/personal/wi21b009_technikum-wien_at/Documents/Dokumente/FH/5. Semester/SEPJ/SEPJ/Backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCCF0537-86AB-4090-9742-8DDAE87698FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{CCCF0537-86AB-4090-9742-8DDAE87698FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1589602-6374-401D-8CE1-05D5C90D930E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{04F9D725-4E7B-4321-9392-CBCBEBAE0302}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Brands" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -597,7 +597,7 @@
   <dimension ref="A1:B68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G100" sqref="G100"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>